<commit_message>
final updates to fish survey protocols
</commit_message>
<xml_diff>
--- a/beach-seines/original_datasheet/marinegeo_datasheet_beach_seines.xlsx
+++ b/beach-seines/original_datasheet/marinegeo_datasheet_beach_seines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\beach-seines\original_datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F642972-FB8F-4988-BA96-89CEF64D8E36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E5AFDB-431F-4F37-8C79-6EA9F6E0CBC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -565,24 +565,90 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -592,9 +658,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -603,75 +666,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,8 +1038,8 @@
   </sheetPr>
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScale="87" zoomScaleNormal="100" zoomScaleSheetLayoutView="98" zoomScalePageLayoutView="87" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A28"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="87" zoomScaleNormal="100" zoomScaleSheetLayoutView="98" zoomScalePageLayoutView="87" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -1062,41 +1059,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="20.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
     </row>
     <row r="2" spans="1:18" ht="33.75" customHeight="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="70" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
       <c r="J2" s="22"/>
       <c r="K2" s="8"/>
       <c r="L2" s="6"/>
@@ -1108,80 +1105,80 @@
       <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" ht="33" customHeight="1">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="58" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="61" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="63"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="42"/>
     </row>
     <row r="4" spans="1:18" ht="33" customHeight="1">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="58" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="37" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="38" t="s">
+      <c r="L4" s="41"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
     </row>
     <row r="5" spans="1:18" ht="12.95" customHeight="1" thickBot="1">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
-      <c r="O5" s="68"/>
-      <c r="P5" s="68"/>
-      <c r="Q5" s="68"/>
-      <c r="R5" s="68"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
     </row>
     <row r="6" spans="1:18" ht="28.5" customHeight="1" thickBot="1">
       <c r="A6" s="3" t="s">
@@ -1190,31 +1187,31 @@
       <c r="B6" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="56"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="43" t="s">
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="55"/>
+      <c r="N6" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="45"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="67"/>
     </row>
     <row r="7" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A7" s="69"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -1234,9 +1231,9 @@
       <c r="R7" s="18"/>
     </row>
     <row r="8" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A8" s="57"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="42"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1254,9 +1251,9 @@
       <c r="R8" s="20"/>
     </row>
     <row r="9" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A9" s="46"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -1276,9 +1273,9 @@
       <c r="R9" s="23"/>
     </row>
     <row r="10" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A10" s="46"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="51"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="62"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -1296,9 +1293,9 @@
       <c r="R10" s="26"/>
     </row>
     <row r="11" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A11" s="57"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1318,9 +1315,9 @@
       <c r="R11" s="18"/>
     </row>
     <row r="12" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A12" s="57"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1338,9 +1335,9 @@
       <c r="R12" s="20"/>
     </row>
     <row r="13" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A13" s="46"/>
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -1360,9 +1357,9 @@
       <c r="R13" s="23"/>
     </row>
     <row r="14" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A14" s="46"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="62"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1380,9 +1377,9 @@
       <c r="R14" s="26"/>
     </row>
     <row r="15" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A15" s="57"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1402,9 +1399,9 @@
       <c r="R15" s="18"/>
     </row>
     <row r="16" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A16" s="57"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1422,9 +1419,9 @@
       <c r="R16" s="20"/>
     </row>
     <row r="17" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A17" s="46"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1444,9 +1441,9 @@
       <c r="R17" s="23"/>
     </row>
     <row r="18" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A18" s="46"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="51"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="62"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1464,9 +1461,9 @@
       <c r="R18" s="26"/>
     </row>
     <row r="19" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A19" s="57"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1486,9 +1483,9 @@
       <c r="R19" s="18"/>
     </row>
     <row r="20" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="57"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1506,9 +1503,9 @@
       <c r="R20" s="20"/>
     </row>
     <row r="21" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A21" s="46"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="53"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -1528,9 +1525,9 @@
       <c r="R21" s="23"/>
     </row>
     <row r="22" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A22" s="46"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="51"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="62"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -1548,9 +1545,9 @@
       <c r="R22" s="26"/>
     </row>
     <row r="23" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A23" s="57"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -1570,9 +1567,9 @@
       <c r="R23" s="18"/>
     </row>
     <row r="24" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A24" s="57"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="42"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -1590,9 +1587,9 @@
       <c r="R24" s="20"/>
     </row>
     <row r="25" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A25" s="46"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="53"/>
+      <c r="A25" s="63"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -1612,9 +1609,9 @@
       <c r="R25" s="23"/>
     </row>
     <row r="26" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A26" s="46"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="51"/>
+      <c r="A26" s="63"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -1632,9 +1629,9 @@
       <c r="R26" s="26"/>
     </row>
     <row r="27" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A27" s="57"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1654,9 +1651,9 @@
       <c r="R27" s="18"/>
     </row>
     <row r="28" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A28" s="57"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="42"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1674,9 +1671,9 @@
       <c r="R28" s="20"/>
     </row>
     <row r="29" spans="1:18" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A29" s="46"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="49"/>
+      <c r="A29" s="63"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="70"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -1696,9 +1693,9 @@
       <c r="R29" s="23"/>
     </row>
     <row r="30" spans="1:18" ht="17.25" customHeight="1">
-      <c r="A30" s="47"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
+      <c r="A30" s="68"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="62"/>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
@@ -1716,9 +1713,9 @@
       <c r="R30" s="30"/>
     </row>
     <row r="31" spans="1:18" ht="18" customHeight="1" thickBot="1">
-      <c r="A31" s="57"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="49"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1738,9 +1735,9 @@
       <c r="R31" s="36"/>
     </row>
     <row r="32" spans="1:18" ht="18" customHeight="1">
-      <c r="A32" s="66"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40"/>
+      <c r="A32" s="47"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
       <c r="D32" s="31"/>
       <c r="E32" s="31"/>
       <c r="F32" s="31"/>
@@ -1758,49 +1755,74 @@
       <c r="R32" s="33"/>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="65"/>
-      <c r="K33" s="65"/>
-      <c r="L33" s="65"/>
-      <c r="M33" s="65"/>
-      <c r="N33" s="65"/>
-      <c r="O33" s="65"/>
-      <c r="P33" s="65"/>
-      <c r="Q33" s="65"/>
-      <c r="R33" s="65"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="44"/>
+      <c r="Q33" s="44"/>
+      <c r="R33" s="44"/>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="72"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
-      <c r="K34" s="72"/>
-      <c r="L34" s="72"/>
-      <c r="M34" s="72"/>
-      <c r="N34" s="72"/>
-      <c r="O34" s="72"/>
-      <c r="P34" s="72"/>
-      <c r="Q34" s="72"/>
-      <c r="R34" s="72"/>
+      <c r="A34" s="45"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="41">
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="B23:C24"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="D6:M6"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="B13:C14"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="K3:R3"/>
@@ -1817,30 +1839,6 @@
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D2:I2"/>
     <mergeCell ref="B21:C22"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="B13:C14"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="B23:C24"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="B27:C28"/>
-    <mergeCell ref="D6:M6"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="98" orientation="portrait" r:id="rId1"/>

</xml_diff>